<commit_message>
Finaly found the best path :)
</commit_message>
<xml_diff>
--- a/DatasetForClustering.xlsx
+++ b/DatasetForClustering.xlsx
@@ -15449,8 +15449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P816"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="M356" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O372" sqref="O372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -17893,9 +17893,6 @@
       <c r="M52" s="7" t="s">
         <v>3694</v>
       </c>
-      <c r="N52" t="b">
-        <v>0</v>
-      </c>
       <c r="O52" t="s">
         <v>3695</v>
       </c>
@@ -33146,9 +33143,6 @@
       </c>
       <c r="N372" t="s">
         <v>4735</v>
-      </c>
-      <c r="O372" t="b">
-        <v>0</v>
       </c>
       <c r="P372" t="s">
         <v>4736</v>

</xml_diff>